<commit_message>
All iOS Store URLs Added
</commit_message>
<xml_diff>
--- a/reviews2.xlsx
+++ b/reviews2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +463,7 @@
         <v>4.8</v>
       </c>
       <c r="D2" t="n">
-        <v>58553</v>
+        <v>58675</v>
       </c>
     </row>
     <row r="3">
@@ -479,7 +479,7 @@
         <v>4.8</v>
       </c>
       <c r="D3" t="n">
-        <v>4066</v>
+        <v>4077</v>
       </c>
     </row>
     <row r="4">
@@ -511,7 +511,7 @@
         <v>4.6</v>
       </c>
       <c r="D5" t="n">
-        <v>376494</v>
+        <v>377323</v>
       </c>
     </row>
     <row r="6">
@@ -527,7 +527,7 @@
         <v>4.6</v>
       </c>
       <c r="D6" t="n">
-        <v>4698161</v>
+        <v>4700977</v>
       </c>
     </row>
     <row r="7">
@@ -543,7 +543,7 @@
         <v>4.5</v>
       </c>
       <c r="D7" t="n">
-        <v>41700</v>
+        <v>41715</v>
       </c>
     </row>
     <row r="8">
@@ -559,7 +559,7 @@
         <v>4.6</v>
       </c>
       <c r="D8" t="n">
-        <v>313588</v>
+        <v>314073</v>
       </c>
     </row>
     <row r="9">
@@ -575,7 +575,7 @@
         <v>4.8</v>
       </c>
       <c r="D9" t="n">
-        <v>2414212</v>
+        <v>2414167</v>
       </c>
     </row>
     <row r="10">
@@ -591,7 +591,7 @@
         <v>4.8</v>
       </c>
       <c r="D10" t="n">
-        <v>42654</v>
+        <v>42656</v>
       </c>
     </row>
     <row r="11">
@@ -607,7 +607,7 @@
         <v>4.7</v>
       </c>
       <c r="D11" t="n">
-        <v>22371</v>
+        <v>22498</v>
       </c>
     </row>
     <row r="12">
@@ -623,7 +623,7 @@
         <v>4.8</v>
       </c>
       <c r="D12" t="n">
-        <v>1909166</v>
+        <v>1913188</v>
       </c>
     </row>
     <row r="13">
@@ -639,7 +639,7 @@
         <v>4.5</v>
       </c>
       <c r="D13" t="n">
-        <v>1047109</v>
+        <v>1047203</v>
       </c>
     </row>
     <row r="14">
@@ -655,7 +655,7 @@
         <v>4.5</v>
       </c>
       <c r="D14" t="n">
-        <v>252884</v>
+        <v>253099</v>
       </c>
     </row>
     <row r="15">
@@ -671,7 +671,7 @@
         <v>4.4</v>
       </c>
       <c r="D15" t="n">
-        <v>112600</v>
+        <v>112693</v>
       </c>
     </row>
     <row r="16">
@@ -687,7 +687,7 @@
         <v>4.4</v>
       </c>
       <c r="D16" t="n">
-        <v>66434</v>
+        <v>66771</v>
       </c>
     </row>
     <row r="17">
@@ -703,7 +703,7 @@
         <v>4.3</v>
       </c>
       <c r="D17" t="n">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18">
@@ -712,14 +712,14 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>myAT&amp;amp;T</t>
+          <t>Spectrum TV</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>4</v>
+        <v>4.7</v>
       </c>
       <c r="D18" t="n">
-        <v>3992454</v>
+        <v>393136</v>
       </c>
     </row>
     <row r="19">
@@ -728,14 +728,14 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Spectrum SportsNet: Live Games</t>
+          <t>myAT&amp;amp;T</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>4.6</v>
+        <v>4</v>
       </c>
       <c r="D19" t="n">
-        <v>3871</v>
+        <v>3992411</v>
       </c>
     </row>
     <row r="20">
@@ -744,14 +744,14 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>MediacomConnect</t>
+          <t>Spectrum SportsNet: Live Games</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3.3</v>
+        <v>4.6</v>
       </c>
       <c r="D20" t="n">
-        <v>6372</v>
+        <v>3895</v>
       </c>
     </row>
     <row r="21">
@@ -760,14 +760,14 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>MyMetro</t>
+          <t>MediacomConnect</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>2.8</v>
+        <v>3.3</v>
       </c>
       <c r="D21" t="n">
-        <v>2906</v>
+        <v>6380</v>
       </c>
     </row>
     <row r="22">
@@ -776,14 +776,270 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
+          <t>MyMetro</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="D22" t="n">
+        <v>2909</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
           <t>MyFrontier</t>
         </is>
       </c>
-      <c r="C22" t="n">
+      <c r="C23" t="n">
         <v>4.4</v>
       </c>
-      <c r="D22" t="n">
-        <v>43314</v>
+      <c r="D23" t="n">
+        <v>43402</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Xfinity</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="D24" t="n">
+        <v>832045</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Google Fiber</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="D25" t="n">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>My Viasat</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1499</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Armstrong</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="D27" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>RCN Mobile</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="D28" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>HughesNet Mobile</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="D29" t="n">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>HT My Account</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="D30" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Midco My Account</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="D31" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Optimum Support</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="D32" t="n">
+        <v>1335</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>UScellular™ – My Account</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="D33" t="n">
+        <v>25203</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>My SECTV</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="D34" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Optimum TV</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="D35" t="n">
+        <v>12430</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Breezeline TV</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="D36" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>My Blue Ridge</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="D37" t="n">
+        <v>3081</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>myBuckeye</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D38" t="n">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>